<commit_message>
Inicio de modulo registro de usuarios
</commit_message>
<xml_diff>
--- a/database/seeds/Imports/Menu.xlsx
+++ b/database/seeds/Imports/Menu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
   <si>
     <t>Catálogos</t>
   </si>
@@ -113,9 +113,6 @@
     <t>permisos</t>
   </si>
   <si>
-    <t>account_tree</t>
-  </si>
-  <si>
     <t>Permisos nuevo</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>roles</t>
   </si>
   <si>
-    <t>all_inbox</t>
-  </si>
-  <si>
     <t>Roles nuevo</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>usuarios-rol</t>
   </si>
   <si>
-    <t>account_box</t>
-  </si>
-  <si>
     <t>Asignar roles usuario</t>
   </si>
   <si>
@@ -225,6 +216,78 @@
   </si>
   <si>
     <t>Digitador</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>usuarios</t>
+  </si>
+  <si>
+    <t>supervisor_account</t>
+  </si>
+  <si>
+    <t>Usuarios nuevo</t>
+  </si>
+  <si>
+    <t>Ruta para crear nuevo usuario</t>
+  </si>
+  <si>
+    <t>Usuarios editar</t>
+  </si>
+  <si>
+    <t>usuarios/editar</t>
+  </si>
+  <si>
+    <t>usuarios/nuevo</t>
+  </si>
+  <si>
+    <t>Ruta para editar un usuario</t>
+  </si>
+  <si>
+    <t>Solicitudes</t>
+  </si>
+  <si>
+    <t>solicitudes</t>
+  </si>
+  <si>
+    <t>Menú para listar todas las solicitudes</t>
+  </si>
+  <si>
+    <t>Solicitudes nueva</t>
+  </si>
+  <si>
+    <t>solicitudes/nuevo</t>
+  </si>
+  <si>
+    <t>assignment</t>
+  </si>
+  <si>
+    <t>Ruta para nueva solicitud</t>
+  </si>
+  <si>
+    <t>Solicitudes editar</t>
+  </si>
+  <si>
+    <t>solicitudes/editar</t>
+  </si>
+  <si>
+    <t>Ruta para editar solicitud</t>
+  </si>
+  <si>
+    <t>Servicios</t>
+  </si>
+  <si>
+    <t>servicios</t>
+  </si>
+  <si>
+    <t>Menú para listar los servicios</t>
+  </si>
+  <si>
+    <t>Menú para listar todos los usuarios</t>
+  </si>
+  <si>
+    <t>style</t>
   </si>
 </sst>
 </file>
@@ -542,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,13 +640,13 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H1">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -600,19 +663,19 @@
         <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -623,11 +686,11 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
@@ -635,13 +698,13 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -652,11 +715,11 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
@@ -664,13 +727,13 @@
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -681,25 +744,25 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -710,10 +773,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -722,13 +785,13 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -739,10 +802,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -751,13 +814,13 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -768,25 +831,25 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -797,10 +860,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -809,13 +872,13 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -838,13 +901,13 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H10">
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -867,13 +930,13 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -896,13 +959,13 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -925,13 +988,13 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -954,13 +1017,13 @@
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H14">
         <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -983,13 +1046,13 @@
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1012,13 +1075,13 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1041,13 +1104,13 @@
         <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H17">
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1070,13 +1133,13 @@
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1099,13 +1162,216 @@
         <v>10</v>
       </c>
       <c r="G19" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s">
         <v>66</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>64</v>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+      <c r="I26" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creación de la vista de pago
</commit_message>
<xml_diff>
--- a/database/seeds/Imports/Menu.xlsx
+++ b/database/seeds/Imports/Menu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
   <si>
     <t>Catálogos</t>
   </si>
@@ -354,6 +354,24 @@
   </si>
   <si>
     <t>Ruta para editar un integrante</t>
+  </si>
+  <si>
+    <t>Pagos nuevo</t>
+  </si>
+  <si>
+    <t>pagos/nuevo</t>
+  </si>
+  <si>
+    <t>Ruta para generar un nuevo pago</t>
+  </si>
+  <si>
+    <t>Pagos detalle</t>
+  </si>
+  <si>
+    <t>pagos/detalle</t>
+  </si>
+  <si>
+    <t>Ruta para el detalle de pagos</t>
   </si>
 </sst>
 </file>
@@ -671,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,6 +1661,64 @@
         <v>109</v>
       </c>
     </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Creando boleta de registro
</commit_message>
<xml_diff>
--- a/database/seeds/Imports/Menu.xlsx
+++ b/database/seeds/Imports/Menu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="132">
   <si>
     <t>Catálogos</t>
   </si>
@@ -372,6 +372,54 @@
   </si>
   <si>
     <t>Ruta para el detalle de pagos</t>
+  </si>
+  <si>
+    <t>Mis servicios</t>
+  </si>
+  <si>
+    <t>mis-servicios</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Menú para visualizar servicios</t>
+  </si>
+  <si>
+    <t>Mis servicios detalle</t>
+  </si>
+  <si>
+    <t>mis-servicios/detalle</t>
+  </si>
+  <si>
+    <t>assignment_ind</t>
+  </si>
+  <si>
+    <t>autorizaciones</t>
+  </si>
+  <si>
+    <t>Submenú para autorizaciones</t>
+  </si>
+  <si>
+    <t>Autorización</t>
+  </si>
+  <si>
+    <t>Autorización nuevo</t>
+  </si>
+  <si>
+    <t>autorizaciones/nuevo</t>
+  </si>
+  <si>
+    <t>Ruta para nueva autorización</t>
+  </si>
+  <si>
+    <t>Autorización editar</t>
+  </si>
+  <si>
+    <t>autorizaciones/editar</t>
+  </si>
+  <si>
+    <t>Rutar para editar autorización</t>
   </si>
 </sst>
 </file>
@@ -689,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,6 +1767,151 @@
         <v>115</v>
       </c>
     </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" t="s">
+        <v>118</v>
+      </c>
+      <c r="H36">
+        <v>7</v>
+      </c>
+      <c r="I36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" t="s">
+        <v>121</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" t="s">
+        <v>118</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>63</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="I38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" t="s">
+        <v>63</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Creando graficas de reportes
</commit_message>
<xml_diff>
--- a/database/seeds/Imports/Menu.xlsx
+++ b/database/seeds/Imports/Menu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="141">
   <si>
     <t>Catálogos</t>
   </si>
@@ -420,6 +420,33 @@
   </si>
   <si>
     <t>Rutar para editar autorización</t>
+  </si>
+  <si>
+    <t>Reportes</t>
+  </si>
+  <si>
+    <t>assessment</t>
+  </si>
+  <si>
+    <t>Gráficos</t>
+  </si>
+  <si>
+    <t>reporte-grafico</t>
+  </si>
+  <si>
+    <t>Submenu para reportes graficos</t>
+  </si>
+  <si>
+    <t>Menu para reportes</t>
+  </si>
+  <si>
+    <t>Documentos</t>
+  </si>
+  <si>
+    <t>reporte-documento</t>
+  </si>
+  <si>
+    <t>Submenu para reportes en documentos</t>
   </si>
 </sst>
 </file>
@@ -737,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,6 +1939,93 @@
         <v>131</v>
       </c>
     </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>133</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H41">
+        <v>8</v>
+      </c>
+      <c r="I41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" t="s">
+        <v>63</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Editar estado de servicio
</commit_message>
<xml_diff>
--- a/database/seeds/Imports/Menu.xlsx
+++ b/database/seeds/Imports/Menu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="148">
   <si>
     <t>Catálogos</t>
   </si>
@@ -447,6 +447,27 @@
   </si>
   <si>
     <t>Submenu para reportes en documentos</t>
+  </si>
+  <si>
+    <t>servicios/editar</t>
+  </si>
+  <si>
+    <t>Ruta para editar estado de servicio</t>
+  </si>
+  <si>
+    <t>Servicios editar</t>
+  </si>
+  <si>
+    <t>Crear respaldo</t>
+  </si>
+  <si>
+    <t>crear-respaldo</t>
+  </si>
+  <si>
+    <t>backup</t>
+  </si>
+  <si>
+    <t>Menú para crear respaldo</t>
   </si>
 </sst>
 </file>
@@ -764,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1084,7 @@
         <v>63</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10" t="s">
         <v>55</v>
@@ -1353,7 +1374,7 @@
         <v>63</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I20" t="s">
         <v>86</v>
@@ -1440,7 +1461,7 @@
         <v>63</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I23" t="s">
         <v>75</v>
@@ -1585,7 +1606,7 @@
         <v>63</v>
       </c>
       <c r="H28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I28" t="s">
         <v>85</v>
@@ -1643,7 +1664,7 @@
         <v>63</v>
       </c>
       <c r="H30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I30" t="s">
         <v>100</v>
@@ -1817,7 +1838,7 @@
         <v>118</v>
       </c>
       <c r="H36">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I36" t="s">
         <v>119</v>
@@ -1962,7 +1983,7 @@
         <v>63</v>
       </c>
       <c r="H41">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I41" t="s">
         <v>137</v>
@@ -2024,6 +2045,64 @@
       </c>
       <c r="I43" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>28</v>
+      </c>
+      <c r="C44" t="s">
+        <v>143</v>
+      </c>
+      <c r="D44" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45" t="s">
+        <v>145</v>
+      </c>
+      <c r="E45" t="s">
+        <v>146</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>